<commit_message>
only integet16 conf designs
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer16/30mhz/mxu_10x10/power.xlsx
+++ b/dtpu_configurations/only_integer16/30mhz/mxu_10x10/power.xlsx
@@ -175,19 +175,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>0.01407705806195736</v>
+        <v>0.014926894567906857</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.005813669878989458</v>
+        <v>0.006258303299546242</v>
       </c>
       <c r="D2" t="n" s="4">
-        <v>0.004318628925830126</v>
+        <v>0.004506985656917095</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>0.0031784577295184135</v>
+        <v>0.003292342182248831</v>
       </c>
       <c r="F2" t="n" s="4">
-        <v>1.8883965822169557E-5</v>
+        <v>2.4721293812035583E-5</v>
       </c>
       <c r="G2" t="n" s="4">
         <v>8.419506484642625E-4</v>
@@ -199,10 +199,10 @@
         <v>1.2575732469558716</v>
       </c>
       <c r="J2" t="n" s="4">
-        <v>0.12725776433944702</v>
+        <v>0.12727078795433044</v>
       </c>
       <c r="K2" t="n" s="4">
-        <v>1.413671612739563</v>
+        <v>1.4152871370315552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>